<commit_message>
add evaluation for topologies and plots
</commit_message>
<xml_diff>
--- a/master_thesis/data/data.xlsx
+++ b/master_thesis/data/data.xlsx
@@ -3,27 +3,33 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DAB517-02F2-4F82-BC80-E9B0B32455FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB297FF5-C42E-4E98-8595-A036BDDB4128}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="synthesis_info_18_0" sheetId="1" r:id="rId1"/>
     <sheet name="syn_inf_18_1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="PCIe info" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Design</t>
   </si>
@@ -62,6 +68,36 @@
   </si>
   <si>
     <t>Frequency 18.1.1 (MHz)</t>
+  </si>
+  <si>
+    <t>Link Speed</t>
+  </si>
+  <si>
+    <t>Lanes</t>
+  </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Peak Bandwidth (GB/s)</t>
+  </si>
+  <si>
+    <t>MPI+PCIe</t>
+  </si>
+  <si>
+    <t>Within Node 1 Channel</t>
+  </si>
+  <si>
+    <t>Within Node 4 Channel</t>
+  </si>
+  <si>
+    <t>Fully Connect</t>
   </si>
 </sst>
 </file>
@@ -661,7 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6E670E-65C3-432C-AB53-BE0F06DD0D57}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -756,12 +792,98 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B913EA-5A35-4C8D-A537-CF335B650397}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <f>40/8</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <f>B2*B3</f>
+        <v>7880</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <f>1/((1/7.88)+(1/12.5)+(1/7.88))</f>
+        <v>2.9957420924574207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>2.9950000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add evaluation for execution runtime
Signed-off-by: Gaurav Kumar Singh <gauravks@mail.uni-paderborn.de>
</commit_message>
<xml_diff>
--- a/master_thesis/data/data.xlsx
+++ b/master_thesis/data/data.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB297FF5-C42E-4E98-8595-A036BDDB4128}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E0BF06-0CBA-4B0E-8ED3-28369DC9C34F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="synthesis_info_18_0" sheetId="1" r:id="rId1"/>
     <sheet name="syn_inf_18_1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="PCIe info" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="PCIe info" sheetId="3" r:id="rId5"/>
+    <sheet name="bandwidths" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="87">
   <si>
     <t>Design</t>
   </si>
   <si>
-    <t>Frequency</t>
-  </si>
-  <si>
     <t>Logic</t>
   </si>
   <si>
@@ -98,6 +99,201 @@
   </si>
   <si>
     <t>Fully Connect</t>
+  </si>
+  <si>
+    <t>Designs</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>Ir-regular</t>
+  </si>
+  <si>
+    <t>Interleaved</t>
+  </si>
+  <si>
+    <t>Non-interleaved</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>MPI N2</t>
+  </si>
+  <si>
+    <t>MPI N4</t>
+  </si>
+  <si>
+    <t>WN 1CH</t>
+  </si>
+  <si>
+    <t>WN 4CH</t>
+  </si>
+  <si>
+    <t>Frequency(with)</t>
+  </si>
+  <si>
+    <t>(Frequency (No-flags))</t>
+  </si>
+  <si>
+    <t>FPGA ONLY 4 CH</t>
+  </si>
+  <si>
+    <t>Value at p = 3</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Computation</t>
+  </si>
+  <si>
+    <t>p_Nfp</t>
+  </si>
+  <si>
+    <t>p_Np</t>
+  </si>
+  <si>
+    <t>p_max_NfpNfaces_Np</t>
+  </si>
+  <si>
+    <t>BSIZE</t>
+  </si>
+  <si>
+    <t>VOL_UNROLL</t>
+  </si>
+  <si>
+    <t>SURF_UNROLL</t>
+  </si>
+  <si>
+    <t>(PFAC*((p_Np+PFAC-1)/PFAC))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max(p_Nfp*p_Nfaces,p_Np) </t>
+  </si>
+  <si>
+    <t>((p + 1)*(p+2)/2)</t>
+  </si>
+  <si>
+    <t>((p + 1)*(p+2)*(p+3)/6)</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>MIDG2 MPI FPGA</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Memory optimization flags</t>
+  </si>
+  <si>
+    <t>Added latency</t>
+  </si>
+  <si>
+    <t>No. FPGAs used</t>
+  </si>
+  <si>
+    <t>Fully connected with IO Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Within Node with 1 IO Channel </t>
+  </si>
+  <si>
+    <t>Within Node with 4 IO Channels</t>
+  </si>
+  <si>
+    <t>Fully Conneted FPGA Only</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>MPI_N2</t>
+  </si>
+  <si>
+    <t>MPI_N4</t>
+  </si>
+  <si>
+    <t>MPI_N2_nf</t>
+  </si>
+  <si>
+    <t>MPI_N4_nf</t>
+  </si>
+  <si>
+    <t>WNIO</t>
+  </si>
+  <si>
+    <t>WNIO_nf</t>
+  </si>
+  <si>
+    <t>FCIO</t>
+  </si>
+  <si>
+    <t>FCIO_nf</t>
+  </si>
+  <si>
+    <t>WNIO_4CH</t>
+  </si>
+  <si>
+    <t>WNIO_4CH_nf</t>
+  </si>
+  <si>
+    <t>FC_nf</t>
+  </si>
+  <si>
+    <t>WN</t>
+  </si>
+  <si>
+    <t>WN_nolat</t>
+  </si>
+  <si>
+    <t>WN_nf</t>
+  </si>
+  <si>
+    <t>WN_nolat_nf</t>
+  </si>
+  <si>
+    <t>FC_nolat</t>
+  </si>
+  <si>
+    <t>FC_nolat_nf</t>
+  </si>
+  <si>
+    <t>Fmax(MHz)</t>
+  </si>
+  <si>
+    <t>18.0.1</t>
+  </si>
+  <si>
+    <t>18.1.1</t>
+  </si>
+  <si>
+    <t>18.1.1_nf</t>
+  </si>
+  <si>
+    <t>WN_4CH</t>
+  </si>
+  <si>
+    <t>Within Node FPGA Only 1 Channel</t>
+  </si>
+  <si>
+    <t>Within Node FPGA Only 4 Channel</t>
+  </si>
+  <si>
+    <t>WN_4CH_nolat</t>
+  </si>
+  <si>
+    <t>WN_4CH_nf</t>
+  </si>
+  <si>
+    <t>WN_4CH_nolat_nf</t>
   </si>
 </sst>
 </file>
@@ -133,12 +329,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,261 +633,400 @@
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
+      <c r="B3">
         <v>312.3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3">
+        <v>283</v>
+      </c>
+      <c r="D3">
+        <v>288.68</v>
+      </c>
+      <c r="E3" s="1">
         <v>0.34</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F3" s="1">
         <v>0.13</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G3" s="1">
         <v>0.11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4">
         <v>281</v>
       </c>
-      <c r="C3">
+      <c r="C4">
+        <v>287.35000000000002</v>
+      </c>
+      <c r="D4">
+        <v>278.86</v>
+      </c>
+      <c r="E4">
         <v>35</v>
       </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>262.5</v>
+      </c>
+      <c r="C5">
+        <v>223.36</v>
+      </c>
+      <c r="D5">
+        <v>244.91</v>
+      </c>
+      <c r="E5">
+        <v>43</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7">
+        <v>254.16</v>
+      </c>
+      <c r="C7">
+        <v>248.75</v>
+      </c>
+      <c r="D7">
+        <v>231.42</v>
+      </c>
+      <c r="E7">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>262.5</v>
-      </c>
-      <c r="C4">
+      <c r="B8">
+        <v>265.32</v>
+      </c>
+      <c r="C8">
+        <v>276.93</v>
+      </c>
+      <c r="D8">
+        <v>254.84</v>
+      </c>
+      <c r="E8">
+        <v>36</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>236.4</v>
+      </c>
+      <c r="C9">
+        <v>239.46</v>
+      </c>
+      <c r="D9">
+        <v>237.41</v>
+      </c>
+      <c r="E9">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>254.16</v>
-      </c>
-      <c r="C5">
-        <v>41</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>265.32</v>
-      </c>
-      <c r="C6">
-        <v>36</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>236.4</v>
-      </c>
-      <c r="C7">
-        <v>43</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E576C-1548-44AE-805E-EAF08E52F2BD}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B7"/>
+      <selection activeCell="B3" sqref="B3:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="2" max="3" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>283</v>
+      </c>
+      <c r="C3">
+        <v>288.68</v>
+      </c>
+      <c r="D3" s="2">
+        <v>26</v>
+      </c>
+      <c r="E3" s="2">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>283</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B4">
+        <v>287.35000000000002</v>
+      </c>
+      <c r="C4">
+        <v>278.86</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
         <v>26</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>223.36</v>
+      </c>
+      <c r="C5">
+        <v>244.91</v>
+      </c>
+      <c r="D5">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>248.75</v>
+      </c>
+      <c r="C7">
+        <v>231.42</v>
+      </c>
+      <c r="D7">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>276.93</v>
+      </c>
+      <c r="C8">
+        <v>254.84</v>
+      </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>239.46</v>
+      </c>
+      <c r="C9">
+        <v>237.41</v>
+      </c>
+      <c r="D9">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <v>37</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
         <v>13</v>
       </c>
-      <c r="E2" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>287.35000000000002</v>
-      </c>
-      <c r="C3">
-        <v>25</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>223.36</v>
-      </c>
-      <c r="C4">
-        <v>28</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>248.75</v>
-      </c>
-      <c r="C5">
-        <v>34</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>276.93</v>
-      </c>
-      <c r="C6">
-        <v>33</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>239.46</v>
-      </c>
-      <c r="C7">
-        <v>36</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>13</v>
+      <c r="I9">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -713,15 +1054,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>312.3</v>
@@ -732,7 +1073,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>281</v>
@@ -743,7 +1084,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>262.5</v>
@@ -754,7 +1095,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>254.16</v>
@@ -765,7 +1106,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>265.32</v>
@@ -776,7 +1117,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>236.4</v>
@@ -791,10 +1132,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C7393E-CBDE-4180-A2BA-B08B69EB0754}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B913EA-5A35-4C8D-A537-CF335B650397}">
   <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8:F12"/>
     </sheetView>
   </sheetViews>
@@ -807,7 +1160,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>985</v>
@@ -815,7 +1168,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -827,7 +1180,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <f>B2*B3</f>
@@ -836,7 +1189,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <f>1/((1/7.88)+(1/12.5)+(1/7.88))</f>
@@ -845,15 +1198,15 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
         <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9">
         <v>2.9950000000000001</v>
@@ -861,7 +1214,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -869,7 +1222,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11">
         <v>20</v>
@@ -877,7 +1230,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12">
         <v>15</v>
@@ -886,4 +1239,622 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FB532B-2642-4AC9-9B9A-01414570E927}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>4.96</v>
+      </c>
+      <c r="C3">
+        <v>4.96</v>
+      </c>
+      <c r="D3">
+        <v>4.96</v>
+      </c>
+      <c r="E3">
+        <v>4.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>19.84</v>
+      </c>
+      <c r="C4">
+        <v>16.41</v>
+      </c>
+      <c r="D4">
+        <v>19.84</v>
+      </c>
+      <c r="E4">
+        <v>16.41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>14.88</v>
+      </c>
+      <c r="C5">
+        <v>14.88</v>
+      </c>
+      <c r="D5">
+        <v>14.88</v>
+      </c>
+      <c r="E5">
+        <v>14.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>1.95</v>
+      </c>
+      <c r="E6">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>1.78</v>
+      </c>
+      <c r="E7">
+        <v>1.76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5693A86C-0414-40E1-B183-BCF0C77CBE75}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE426B-52D5-451C-8A54-F66456905908}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
intermediate after updating for comments
Signed-off-by: Gaurav Kumar Singh <gauravks@mail.uni-paderborn.de>
</commit_message>
<xml_diff>
--- a/master_thesis/data/data.xlsx
+++ b/master_thesis/data/data.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9852033A-222E-4135-B330-F7E8FE324ADF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06815FF0-FB0D-4820-A7D9-42D1864F1632}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="synthesis_info_18_0" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet7" sheetId="11" r:id="rId2"/>
-    <sheet name="syn_inf_18_1" sheetId="2" r:id="rId3"/>
+    <sheet name="syn_inf_18_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet7" sheetId="11" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
     <sheet name="PCIe info" sheetId="3" r:id="rId6"/>
@@ -20,6 +20,7 @@
     <sheet name="Sheet5" sheetId="9" r:id="rId10"/>
     <sheet name="Sheet6" sheetId="10" r:id="rId11"/>
     <sheet name="Sheet8" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet9" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="150">
   <si>
     <t>Design</t>
   </si>
@@ -184,9 +185,6 @@
   </si>
   <si>
     <t>MIDG2 MPI FPGA</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
   <si>
     <t>Memory optimization flags</t>
@@ -447,6 +445,51 @@
   </si>
   <si>
     <t>Memory/Channel operation</t>
+  </si>
+  <si>
+    <t>Arithemetic intensity</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Total Operation</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Toolchain</t>
+  </si>
+  <si>
+    <t>Synthethic Test</t>
+  </si>
+  <si>
+    <t>4Nf · 61</t>
+  </si>
+  <si>
+    <t>N · 4Nf · 12</t>
+  </si>
+  <si>
+    <t>N2 · 36</t>
+  </si>
+  <si>
+    <t>N · 72</t>
   </si>
 </sst>
 </file>
@@ -482,9 +525,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -492,25 +534,29 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,38 +849,29 @@
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -847,19 +884,10 @@
       <c r="D3">
         <v>288.68</v>
       </c>
-      <c r="E3" s="1">
-        <v>0.34</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.13</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>281</v>
@@ -870,19 +898,10 @@
       <c r="D4">
         <v>278.86</v>
       </c>
-      <c r="E4">
-        <v>35</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>262.5</v>
@@ -893,19 +912,10 @@
       <c r="D5">
         <v>244.91</v>
       </c>
-      <c r="E5">
-        <v>43</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>223.01</v>
@@ -917,9 +927,9 @@
         <v>257.26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7">
         <v>254.16</v>
@@ -930,17 +940,8 @@
       <c r="D7">
         <v>231.42</v>
       </c>
-      <c r="E7">
-        <v>41</v>
-      </c>
-      <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -953,17 +954,8 @@
       <c r="D8">
         <v>254.84</v>
       </c>
-      <c r="E8">
-        <v>36</v>
-      </c>
-      <c r="F8">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -976,19 +968,226 @@
       <c r="D9">
         <v>237.41</v>
       </c>
-      <c r="E9">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1">
+        <v>34</v>
+      </c>
+      <c r="I17" s="1">
+        <v>13</v>
+      </c>
+      <c r="J17" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18">
+        <v>35</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19">
         <v>43</v>
       </c>
-      <c r="F9">
-        <v>12</v>
-      </c>
-      <c r="G9">
+      <c r="I19">
+        <v>12</v>
+      </c>
+      <c r="J19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20">
+        <v>41</v>
+      </c>
+      <c r="I20">
+        <v>12</v>
+      </c>
+      <c r="J20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21">
+        <v>41</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="J21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>36</v>
+      </c>
+      <c r="I22">
+        <v>12</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>43</v>
+      </c>
+      <c r="I23">
+        <v>12</v>
+      </c>
+      <c r="J23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L26" t="s">
+        <v>79</v>
+      </c>
+      <c r="M26" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>34</v>
+      </c>
+      <c r="I27">
+        <v>35</v>
+      </c>
+      <c r="J27">
+        <v>43</v>
+      </c>
+      <c r="K27">
+        <v>41</v>
+      </c>
+      <c r="L27">
+        <v>41</v>
+      </c>
+      <c r="M27">
+        <v>36</v>
+      </c>
+      <c r="N27">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1">
+        <v>13</v>
+      </c>
+      <c r="I28">
+        <v>12</v>
+      </c>
+      <c r="J28">
+        <v>12</v>
+      </c>
+      <c r="K28">
+        <v>12</v>
+      </c>
+      <c r="L28">
+        <v>12</v>
+      </c>
+      <c r="M28">
+        <v>12</v>
+      </c>
+      <c r="N28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1">
+        <v>11</v>
+      </c>
+      <c r="I29">
+        <v>11</v>
+      </c>
+      <c r="J29">
+        <v>13</v>
+      </c>
+      <c r="K29">
+        <v>13</v>
+      </c>
+      <c r="L29">
+        <v>11</v>
+      </c>
+      <c r="M29">
+        <v>10</v>
+      </c>
+      <c r="N29">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1011,20 +1210,20 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="11"/>
       <c r="B2">
         <v>3</v>
       </c>
@@ -1202,39 +1401,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="4">
+        <v>91</v>
+      </c>
+      <c r="B2" s="3">
         <v>2753000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="4">
+        <v>92</v>
+      </c>
+      <c r="B3" s="3">
         <v>933120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="5">
+        <v>88</v>
+      </c>
+      <c r="B4" s="4">
         <v>11721</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5">
         <v>229</v>
@@ -1242,7 +1441,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -1252,7 +1451,7 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>5760</v>
       </c>
     </row>
@@ -1266,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042067CC-D924-41A2-9D99-7D44CE28E009}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1283,53 +1482,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>99</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="C3">
         <v>49.28</v>
@@ -1351,10 +1550,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="9"/>
+      <c r="A4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="12"/>
       <c r="C4">
         <v>58.31</v>
       </c>
@@ -1376,9 +1575,9 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="9"/>
+        <v>104</v>
+      </c>
+      <c r="B5" s="12"/>
       <c r="C5">
         <v>47.13</v>
       </c>
@@ -1400,9 +1599,9 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="B6" s="12"/>
       <c r="C6">
         <v>97.9</v>
       </c>
@@ -1424,10 +1623,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="10" t="s">
         <v>106</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="C7">
         <v>0.01</v>
@@ -1450,9 +1649,9 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="10"/>
+        <v>107</v>
+      </c>
+      <c r="B8" s="13"/>
       <c r="C8">
         <v>0.01</v>
       </c>
@@ -1474,9 +1673,9 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="10"/>
+        <v>108</v>
+      </c>
+      <c r="B9" s="13"/>
       <c r="C9">
         <v>1.05</v>
       </c>
@@ -1498,10 +1697,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="10" t="s">
         <v>110</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="C10">
         <v>53.13</v>
@@ -1524,9 +1723,9 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="10"/>
+        <v>111</v>
+      </c>
+      <c r="B11" s="13"/>
       <c r="C11">
         <v>4.8899999999999997</v>
       </c>
@@ -1547,11 +1746,11 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>118</v>
+      <c r="A12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="C12">
         <v>73.37</v>
@@ -1573,10 +1772,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="10"/>
+      <c r="A13" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="13"/>
       <c r="C13">
         <v>45.38</v>
       </c>
@@ -1598,9 +1797,9 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="10"/>
+        <v>114</v>
+      </c>
+      <c r="B14" s="13"/>
       <c r="C14">
         <v>40.51</v>
       </c>
@@ -1622,9 +1821,9 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B15" s="10"/>
+        <v>115</v>
+      </c>
+      <c r="B15" s="13"/>
       <c r="C15">
         <v>40.51</v>
       </c>
@@ -1646,9 +1845,9 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" s="10"/>
+        <v>116</v>
+      </c>
+      <c r="B16" s="13"/>
       <c r="C16">
         <v>0</v>
       </c>
@@ -1669,11 +1868,11 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>126</v>
+      <c r="A17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="C17">
         <v>67.680000000000007</v>
@@ -1695,24 +1894,24 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="12" t="s">
-        <v>125</v>
+      <c r="A18" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="D18">
         <v>60.14</v>
       </c>
       <c r="E18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F18">
         <v>56.9</v>
       </c>
       <c r="G18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H18">
         <v>12862.8</v>
@@ -1720,9 +1919,9 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="10"/>
+        <v>122</v>
+      </c>
+      <c r="B19" s="13"/>
       <c r="C19">
         <v>0.03</v>
       </c>
@@ -1744,9 +1943,9 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="10"/>
+        <v>123</v>
+      </c>
+      <c r="B20" s="13"/>
       <c r="C20">
         <v>0.03</v>
       </c>
@@ -1768,9 +1967,9 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>121</v>
-      </c>
-      <c r="B21" s="10"/>
+        <v>120</v>
+      </c>
+      <c r="B21" s="13"/>
       <c r="C21">
         <v>32.56</v>
       </c>
@@ -1792,9 +1991,9 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="10"/>
+        <v>121</v>
+      </c>
+      <c r="B22" s="13"/>
       <c r="C22">
         <v>32.56</v>
       </c>
@@ -1816,10 +2015,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="C23">
         <v>0.01</v>
@@ -1842,9 +2041,9 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="B24" s="13"/>
       <c r="C24">
         <v>8.2899999999999991</v>
       </c>
@@ -1866,9 +2065,9 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>129</v>
-      </c>
-      <c r="B25" s="10"/>
+        <v>128</v>
+      </c>
+      <c r="B25" s="13"/>
       <c r="C25">
         <v>0.01</v>
       </c>
@@ -1890,9 +2089,9 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="10"/>
+        <v>133</v>
+      </c>
+      <c r="B26" s="13"/>
       <c r="C26">
         <v>0.74</v>
       </c>
@@ -1914,10 +2113,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" s="10" t="s">
         <v>131</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="C27">
         <v>66.739999999999995</v>
@@ -1940,9 +2139,9 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B28" s="10"/>
+        <v>132</v>
+      </c>
+      <c r="B28" s="13"/>
       <c r="C28">
         <v>3.47</v>
       </c>
@@ -1969,36 +2168,189 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9E572C-DEFF-4F9A-AE8C-5349818A2CAE}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A0F99B2-D830-4A06-9EA6-873652ECA13B}">
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5">
+        <f>20*20*36</f>
+        <v>14400</v>
+      </c>
+      <c r="C5">
+        <f>20*6+9</f>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6">
+        <f>20*72</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f>B5+B6</f>
+        <v>15840</v>
+      </c>
+      <c r="D7">
+        <f>B7/(C5*4)</f>
+        <v>30.697674418604652</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10">
+        <f>2*3+3*3+5*2+6*6</f>
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <f>B10*40</f>
+        <v>2440</v>
+      </c>
+      <c r="D10">
+        <f>(40*2+40*12+40*5)</f>
+        <v>760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11">
+        <f>8*6</f>
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <f>B11*20*10</f>
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f>C10+C11</f>
+        <v>12040</v>
+      </c>
+      <c r="E12">
+        <f>C12/(D10*4)</f>
+        <v>3.9605263157894739</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <f>D15+D10+C5</f>
+        <v>894</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f>C15/(D15*4)</f>
+        <v>0.3</v>
+      </c>
+      <c r="F16">
+        <f>C15/(E15*4)</f>
+        <v>1.6778523489932886E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <f>16*5</f>
+        <v>80</v>
+      </c>
+      <c r="D18">
+        <f>5*4*16</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f>C18/D18</f>
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E576C-1548-44AE-805E-EAF08E52F2BD}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2037,22 +2389,22 @@
       <c r="C3">
         <v>288.68</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>26</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>27</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>13</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>13</v>
       </c>
-      <c r="H3" s="2">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="H3" s="1">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1">
         <v>12</v>
       </c>
     </row>
@@ -2121,7 +2473,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>248.75</v>
@@ -2206,7 +2558,406 @@
         <v>12</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1">
+        <v>13</v>
+      </c>
+      <c r="G15" s="1">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1">
+        <v>12</v>
+      </c>
+      <c r="I15" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>26</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>28</v>
+      </c>
+      <c r="E17">
+        <v>30</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19">
+        <v>34</v>
+      </c>
+      <c r="E19">
+        <v>34</v>
+      </c>
+      <c r="F19">
+        <v>12</v>
+      </c>
+      <c r="G19">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>33</v>
+      </c>
+      <c r="F20">
+        <v>12</v>
+      </c>
+      <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>11</v>
+      </c>
+      <c r="I20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>37</v>
+      </c>
+      <c r="F21">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <v>13</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9E572C-DEFF-4F9A-AE8C-5349818A2CAE}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="1">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>27</v>
+      </c>
+      <c r="G3">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>33</v>
+      </c>
+      <c r="I3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="1">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>43</v>
+      </c>
+      <c r="F4">
+        <v>41</v>
+      </c>
+      <c r="G4">
+        <v>41</v>
+      </c>
+      <c r="H4">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="1">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2230,10 +2981,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2365,7 +3116,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5">
@@ -2434,20 +3185,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="11"/>
       <c r="B2" t="s">
         <v>25</v>
       </c>
@@ -2645,13 +3396,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE426B-52D5-451C-8A54-F66456905908}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" customWidth="1"/>
@@ -2659,367 +3410,433 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
-        <v>49</v>
+      <c r="F1" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
         <v>58</v>
       </c>
-      <c r="E2" t="s">
-        <v>59</v>
+      <c r="F2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="10"/>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="10"/>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="10"/>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>54</v>
+      <c r="A6" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="10"/>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>55</v>
+      <c r="A8" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="A9" s="10"/>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>53</v>
+      <c r="A10" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="10"/>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>81</v>
+      <c r="A12" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="10"/>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="10"/>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="10"/>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>82</v>
+      <c r="A16" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
       <c r="B21">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
       <c r="B22">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
       <c r="B23">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="F23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>